<commit_message>
added SLF for all performance groups
</commit_message>
<xml_diff>
--- a/client/Database.xlsx
+++ b/client/Database.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SLFGenerator\client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCB5BE6-5215-4384-8056-DE5319A8CF7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E619AA4A-7252-4DA1-B2FC-686BC7F1A422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97BE9DF7-DD94-4053-A8FF-28E085CB9A4F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{97BE9DF7-DD94-4053-A8FF-28E085CB9A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="120">
   <si>
     <t>ID</t>
   </si>
@@ -156,6 +158,240 @@
   </si>
   <si>
     <t>Generic-Acceleration</t>
+  </si>
+  <si>
+    <t>B1033.013a</t>
+  </si>
+  <si>
+    <t>B1031.001</t>
+  </si>
+  <si>
+    <t>B1031.021a</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>per 100m2</t>
+  </si>
+  <si>
+    <t>EDP</t>
+  </si>
+  <si>
+    <t>DS2</t>
+  </si>
+  <si>
+    <t>DS3</t>
+  </si>
+  <si>
+    <t>DS4</t>
+  </si>
+  <si>
+    <t>DS5</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>B2011.011a</t>
+  </si>
+  <si>
+    <t>C1011.001a</t>
+  </si>
+  <si>
+    <t>C2011.001b</t>
+  </si>
+  <si>
+    <t>C3032.001a</t>
+  </si>
+  <si>
+    <t>D2021.011a</t>
+  </si>
+  <si>
+    <t>D2022.011a</t>
+  </si>
+  <si>
+    <t>D2031.011b</t>
+  </si>
+  <si>
+    <t>D3041.001a</t>
+  </si>
+  <si>
+    <t>D3041.031a</t>
+  </si>
+  <si>
+    <t>D3041.041a</t>
+  </si>
+  <si>
+    <t>D4011.021a</t>
+  </si>
+  <si>
+    <t>D5012.033b</t>
+  </si>
+  <si>
+    <t>E2022.001</t>
+  </si>
+  <si>
+    <t>E2022.023</t>
+  </si>
+  <si>
+    <t>E2022.102a</t>
+  </si>
+  <si>
+    <t>E2022.103a</t>
+  </si>
+  <si>
+    <t>E2022.104a</t>
+  </si>
+  <si>
+    <t>E2022.105a</t>
+  </si>
+  <si>
+    <t>E2022.106a</t>
+  </si>
+  <si>
+    <t>E2022.112a</t>
+  </si>
+  <si>
+    <t>E2022.114a</t>
+  </si>
+  <si>
+    <t>E2022.124a</t>
+  </si>
+  <si>
+    <t>D1014.021</t>
+  </si>
+  <si>
+    <t>D5092.011a</t>
+  </si>
+  <si>
+    <t>D5092.021a</t>
+  </si>
+  <si>
+    <t>D5011.011b</t>
+  </si>
+  <si>
+    <t>D5012.021a</t>
+  </si>
+  <si>
+    <t>D5092.032b</t>
+  </si>
+  <si>
+    <t>D3031.012e</t>
+  </si>
+  <si>
+    <t>D3052.011d</t>
+  </si>
+  <si>
+    <t>100SF</t>
+  </si>
+  <si>
+    <t>1EA</t>
+  </si>
+  <si>
+    <t>250SF</t>
+  </si>
+  <si>
+    <t>1000LF</t>
+  </si>
+  <si>
+    <t>10EA</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Fragilities DS1</t>
+  </si>
+  <si>
+    <t>Cost  DS1</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>CFM</t>
+  </si>
+  <si>
+    <t>KVA</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>Linear foot</t>
+  </si>
+  <si>
+    <t>Square foot</t>
+  </si>
+  <si>
+    <t>cubic feet per minute</t>
+  </si>
+  <si>
+    <t>each</t>
+  </si>
+  <si>
+    <t>kilovolt amper</t>
+  </si>
+  <si>
+    <t>best fit</t>
+  </si>
+  <si>
+    <t>lognormal</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>1 usd = 0.88 euro</t>
+  </si>
+  <si>
+    <t>no scaling for specific country</t>
+  </si>
+  <si>
+    <t>no correction against double counting</t>
+  </si>
+  <si>
+    <t>this is just a pure demonstration</t>
+  </si>
+  <si>
+    <t>1300SF</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Units?</t>
+  </si>
+  <si>
+    <t>Units in cost summary and fragility summary differ sometimes, have you noticed?</t>
+  </si>
+  <si>
+    <t>Me using the means and CVs as it is, does it make sense, or I need to make some modifications?</t>
+  </si>
+  <si>
+    <t>normal truncated</t>
+  </si>
+  <si>
+    <t>luxury content per Greece</t>
+  </si>
+  <si>
+    <t>Why repair cost at higher DS is sometimes lower</t>
+  </si>
+  <si>
+    <t>Total quantity</t>
   </si>
 </sst>
 </file>
@@ -192,10 +428,48 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -204,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -214,6 +488,28 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{782EE2B5-8FE3-4D5C-8CD0-B4042A47447B}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,4 +1534,1996 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B52AD20-FC57-4B76-8A23-C938B11C5479}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="30.42578125" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E268B3A-2F17-40E8-A169-0BB8D9CF87F7}">
+  <dimension ref="A1:AF37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18:H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="11"/>
+    <col min="3" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.140625" style="11"/>
+    <col min="8" max="16" width="9.140625" style="4"/>
+    <col min="17" max="17" width="9.140625" style="11"/>
+    <col min="18" max="31" width="9.140625" style="4"/>
+    <col min="32" max="32" width="9.140625" style="11"/>
+    <col min="33" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="9"/>
+    </row>
+    <row r="2" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" s="10"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="4">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="D3" s="4">
+        <f>C3*7</f>
+        <v>69.72</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.04</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T3" s="4">
+        <f>0.88*12100</f>
+        <v>10648</v>
+      </c>
+      <c r="U3" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="W3" s="4">
+        <f>12400*0.88</f>
+        <v>10912</v>
+      </c>
+      <c r="X3" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z3" s="4">
+        <f>12300*0.88</f>
+        <v>10824</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D37" si="0">C4*7</f>
+        <v>5.32</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>0</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="8">
+        <f>9450*0.88</f>
+        <v>8316</v>
+      </c>
+      <c r="U4" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="W4" s="8">
+        <f>11200*0.88</f>
+        <v>9856</v>
+      </c>
+      <c r="X4" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF4" s="11"/>
+    </row>
+    <row r="5" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>3.9200000000000004</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="12">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="I5" s="7">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1.67E-2</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="M5" s="7">
+        <v>2.23E-2</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="Q5" s="12">
+        <f>30900*0.88</f>
+        <v>27192</v>
+      </c>
+      <c r="R5" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="T5" s="7">
+        <f>37800*0.88</f>
+        <v>33264</v>
+      </c>
+      <c r="U5" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="V5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="W5" s="7">
+        <f>39400*0.88</f>
+        <v>34672</v>
+      </c>
+      <c r="X5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="Y5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z5" s="7">
+        <f>39400*0.88</f>
+        <v>34672</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF5" s="12"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8.52</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>59.64</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="Q6" s="11">
+        <f>3140*0.88</f>
+        <v>2763.2</v>
+      </c>
+      <c r="R6" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T6" s="4">
+        <f>3740*0.88</f>
+        <v>3291.2</v>
+      </c>
+      <c r="U6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K7" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Q7" s="11">
+        <f>1800*0.88</f>
+        <v>1584</v>
+      </c>
+      <c r="R7" s="4">
+        <v>0.48</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="T7" s="4">
+        <f>4300*0.88</f>
+        <v>3784</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="W7" s="4">
+        <f>8990*0.88</f>
+        <v>7911.2</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.05</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="Q8" s="11">
+        <f>1960*0.88</f>
+        <v>1724.8</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="T8" s="4">
+        <f>5500*0.88</f>
+        <v>4840</v>
+      </c>
+      <c r="U8" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="W8" s="4">
+        <f>19800*0.88</f>
+        <v>17424</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1.62</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>11.34</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="11">
+        <v>1.17</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.58</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1.82</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="Q9" s="11">
+        <f>354*0.88</f>
+        <v>311.52</v>
+      </c>
+      <c r="R9" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="T9" s="4">
+        <f>2760*0.88</f>
+        <v>2428.8000000000002</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0.52</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="W9" s="4">
+        <f>5970*0.88</f>
+        <v>5253.6</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q10" s="11">
+        <f>279*0.88</f>
+        <v>245.52</v>
+      </c>
+      <c r="R10" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T10" s="4">
+        <f>2600*0.88</f>
+        <v>2288</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>4.1299999999999996E-2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q11" s="11">
+        <f>279*0.88</f>
+        <v>245.52</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T11" s="4">
+        <f>2600*0.88</f>
+        <v>2288</v>
+      </c>
+      <c r="U11" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q12" s="11">
+        <f>406*0.88</f>
+        <v>357.28000000000003</v>
+      </c>
+      <c r="R12" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T12" s="4">
+        <f>2820*0.88</f>
+        <v>2481.6</v>
+      </c>
+      <c r="U12" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1.92</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q13" s="11">
+        <f>7340*0.88</f>
+        <v>6459.2</v>
+      </c>
+      <c r="R13" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T13" s="4">
+        <f>27700*0.88</f>
+        <v>24376</v>
+      </c>
+      <c r="U13" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.97</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>6.79</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q14" s="11">
+        <f>2830*0.88</f>
+        <v>2490.4</v>
+      </c>
+      <c r="R14" s="4">
+        <v>0.21</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.76</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>5.32</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q15" s="11">
+        <f>14800*0.88</f>
+        <v>13024</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q16" s="11">
+        <f>348*0.88</f>
+        <v>306.24</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T16" s="4">
+        <f>2600*0.88</f>
+        <v>2288</v>
+      </c>
+      <c r="U16" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>1.1900000000000002</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="12">
+        <v>3.05</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="Q17" s="12">
+        <f>9710*0.88</f>
+        <v>8544.7999999999993</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF17" s="12"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6.05</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>42.35</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>200</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4.26</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="0"/>
+        <v>29.82</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>140</v>
+      </c>
+      <c r="R19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="0"/>
+        <v>31.360000000000003</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>600</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="4">
+        <v>4.37</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>30.59</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.42</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>120</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>80</v>
+      </c>
+      <c r="R22" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>3.08</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>100</v>
+      </c>
+      <c r="R23" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.39</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="11">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>140</v>
+      </c>
+      <c r="R24" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>170</v>
+      </c>
+      <c r="R25" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="4">
+        <v>9.61</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="0"/>
+        <v>67.27</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.66</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="11">
+        <v>0.251</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>200</v>
+      </c>
+      <c r="R26" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.07</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="0"/>
+        <v>7.49</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q27" s="11">
+        <v>70</v>
+      </c>
+      <c r="R27" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>3.4299999999999997</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.41</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="11">
+        <v>0.498</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>80</v>
+      </c>
+      <c r="R28" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999995</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.37</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="Q29" s="12">
+        <v>70</v>
+      </c>
+      <c r="R29" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF29" s="12"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="0"/>
+        <v>0.46900000000000003</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="L30" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="Q30" s="11">
+        <f>868*0.88</f>
+        <v>763.84</v>
+      </c>
+      <c r="R30" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T30" s="4">
+        <f>7630*0.88</f>
+        <v>6714.4</v>
+      </c>
+      <c r="U30" s="4">
+        <v>0.32</v>
+      </c>
+      <c r="V30" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="W30" s="4">
+        <f>10700*0.88</f>
+        <v>9416</v>
+      </c>
+      <c r="X30" s="4">
+        <v>0.44</v>
+      </c>
+      <c r="Y30" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z30" s="4">
+        <f>2540*0.88</f>
+        <v>2235.1999999999998</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="AB30" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="0"/>
+        <v>0.126</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="11">
+        <v>0.43</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="Q31" s="11">
+        <f>158000*0.88</f>
+        <v>139040</v>
+      </c>
+      <c r="R31" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.182</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="Q32" s="11">
+        <f>2070*0.88</f>
+        <v>1821.6</v>
+      </c>
+      <c r="R32" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="S32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="T32" s="8">
+        <f>192000*0.88</f>
+        <v>168960</v>
+      </c>
+      <c r="U32" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="V32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF32" s="11"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="0"/>
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="11">
+        <v>1.01</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="Q33" s="11">
+        <f>25200*0.88</f>
+        <v>22176</v>
+      </c>
+      <c r="R33" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="4">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="0"/>
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="11">
+        <v>1.28</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q34" s="11">
+        <f>9710*0.88</f>
+        <v>8544.7999999999993</v>
+      </c>
+      <c r="R34" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="0"/>
+        <v>0.46900000000000003</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="K35" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L35" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="Q35" s="11">
+        <f>12300*0.88</f>
+        <v>10824</v>
+      </c>
+      <c r="R35" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T35" s="4">
+        <f>683*0.88</f>
+        <v>601.04</v>
+      </c>
+      <c r="U35" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="W35" s="4">
+        <f>3170*0.88</f>
+        <v>2789.6</v>
+      </c>
+      <c r="X35" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="Y35" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="0"/>
+        <v>0.46900000000000003</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="11">
+        <v>1.07</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="I36" s="4">
+        <v>1.07</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="Q36" s="11">
+        <f>767*0.88</f>
+        <v>674.96</v>
+      </c>
+      <c r="R36" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="T36" s="4">
+        <f>12200*0.88</f>
+        <v>10736</v>
+      </c>
+      <c r="U36" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="V36" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="0"/>
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="12">
+        <v>1.07</v>
+      </c>
+      <c r="H37" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I37" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="L37" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="M37" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="N37" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="Q37" s="12">
+        <f>207*0.88</f>
+        <v>182.16</v>
+      </c>
+      <c r="R37" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="T37" s="7">
+        <f>2580*0.88</f>
+        <v>2270.4</v>
+      </c>
+      <c r="U37" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="W37" s="7">
+        <f>519*0.88</f>
+        <v>456.72</v>
+      </c>
+      <c r="X37" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="Y37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z37" s="7">
+        <f>519*0.88</f>
+        <v>456.72</v>
+      </c>
+      <c r="AA37" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="AB37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF37" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>